<commit_message>
Negative Test Cases on Source Demo
</commit_message>
<xml_diff>
--- a/TestData/Login.xlsx
+++ b/TestData/Login.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CorrectData" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="IncorrectData" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -38,6 +39,27 @@
   </si>
   <si>
     <t xml:space="preserve">performance_glitch_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a12365561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard_user  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  problem_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">performance_glitch_ user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secret_sauce  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a123</t>
   </si>
 </sst>
 </file>
@@ -150,11 +172,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.67"/>
   </cols>
@@ -200,4 +222,87 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.26"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>